<commit_message>
Support RKA and RKT arcs in strategic model
</commit_message>
<xml_diff>
--- a/pareto/tests/strategic_small_case_study_load_removaleff.xlsx
+++ b/pareto/tests/strategic_small_case_study_load_removaleff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089CE096-EC15-48B1-B6C8-83BE79DDD390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAFD3A5-AAFF-4870-9276-6BE85440D687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="88" activeTab="93" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -47,73 +47,72 @@
     <sheet name="SCA" sheetId="97" r:id="rId32"/>
     <sheet name="RNA" sheetId="62" r:id="rId33"/>
     <sheet name="ROA" sheetId="122" r:id="rId34"/>
-    <sheet name="PCT" sheetId="42" r:id="rId35"/>
-    <sheet name="FCT" sheetId="70" r:id="rId36"/>
-    <sheet name="PKT" sheetId="43" r:id="rId37"/>
-    <sheet name="CKT" sheetId="44" r:id="rId38"/>
-    <sheet name="CCT" sheetId="74" r:id="rId39"/>
-    <sheet name="CST" sheetId="64" r:id="rId40"/>
-    <sheet name="RST" sheetId="123" r:id="rId41"/>
-    <sheet name="ROT" sheetId="124" r:id="rId42"/>
-    <sheet name="SOT" sheetId="125" r:id="rId43"/>
-    <sheet name="Elevation" sheetId="117" r:id="rId44"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId45"/>
-    <sheet name="PadRates" sheetId="65" r:id="rId46"/>
-    <sheet name="FlowbackRates" sheetId="75" r:id="rId47"/>
-    <sheet name="WellPressure" sheetId="118" r:id="rId48"/>
-    <sheet name="InitialPipelineCapacity" sheetId="66" r:id="rId49"/>
-    <sheet name="InitialPipelineDiameters" sheetId="119" r:id="rId50"/>
-    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId51"/>
-    <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId52"/>
-    <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId53"/>
-    <sheet name="ReuseMinimum" sheetId="126" r:id="rId54"/>
-    <sheet name="ReuseCapacity" sheetId="127" r:id="rId55"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId56"/>
-    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId57"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId58"/>
-    <sheet name="NodeCapacities" sheetId="107" r:id="rId59"/>
-    <sheet name="DisposalOperatingCapacity" sheetId="111" r:id="rId60"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId61"/>
-    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId62"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId63"/>
-    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId64"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId65"/>
-    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId66"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId67"/>
-    <sheet name="DisposalExpansionCost" sheetId="90" r:id="rId68"/>
-    <sheet name="DisposalCapacityIncrements" sheetId="79" r:id="rId69"/>
-    <sheet name="StorageExpansionCost" sheetId="91" r:id="rId70"/>
-    <sheet name="StorageCapacityIncrements" sheetId="81" r:id="rId71"/>
-    <sheet name="TreatmentExpansionCost" sheetId="92" r:id="rId72"/>
-    <sheet name="TreatmentCapacityIncrements" sheetId="87" r:id="rId73"/>
-    <sheet name="PipelineCapexDistanceBased" sheetId="89" r:id="rId74"/>
-    <sheet name="PipelineExpansionDistance" sheetId="103" r:id="rId75"/>
-    <sheet name="PipelineCapexCapacityBased" sheetId="101" r:id="rId76"/>
-    <sheet name="PipelineCapacityIncrements" sheetId="100" r:id="rId77"/>
-    <sheet name="PipelineDiameterValues" sheetId="93" r:id="rId78"/>
-    <sheet name="TreatmentEfficiency" sheetId="85" r:id="rId79"/>
-    <sheet name="RemovalEfficiency" sheetId="116" r:id="rId80"/>
-    <sheet name="DesalinationTechnologies" sheetId="112" r:id="rId81"/>
-    <sheet name="DesalinationSites" sheetId="114" r:id="rId82"/>
-    <sheet name="BeneficialReuseCredit" sheetId="128" r:id="rId83"/>
-    <sheet name="CompletionsPadOutsideSystem" sheetId="113" r:id="rId84"/>
-    <sheet name="Hydraulics" sheetId="95" r:id="rId85"/>
-    <sheet name="Economics" sheetId="99" r:id="rId86"/>
-    <sheet name="PadWaterQuality" sheetId="104" r:id="rId87"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="105" r:id="rId88"/>
-    <sheet name="PadStorageInitialWaterQuality" sheetId="106" r:id="rId89"/>
-    <sheet name="TreatmentExpansionLeadTime" sheetId="129" r:id="rId90"/>
-    <sheet name="DisposalExpansionLeadTime" sheetId="130" r:id="rId91"/>
-    <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId92"/>
-    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId93"/>
-    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId94"/>
+    <sheet name="RKA" sheetId="134" r:id="rId35"/>
+    <sheet name="PCT" sheetId="42" r:id="rId36"/>
+    <sheet name="FCT" sheetId="70" r:id="rId37"/>
+    <sheet name="PKT" sheetId="43" r:id="rId38"/>
+    <sheet name="CKT" sheetId="44" r:id="rId39"/>
+    <sheet name="CCT" sheetId="74" r:id="rId40"/>
+    <sheet name="CST" sheetId="64" r:id="rId41"/>
+    <sheet name="RST" sheetId="123" r:id="rId42"/>
+    <sheet name="ROT" sheetId="124" r:id="rId43"/>
+    <sheet name="SOT" sheetId="125" r:id="rId44"/>
+    <sheet name="RKT" sheetId="135" r:id="rId45"/>
+    <sheet name="Elevation" sheetId="117" r:id="rId46"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId47"/>
+    <sheet name="PadRates" sheetId="65" r:id="rId48"/>
+    <sheet name="FlowbackRates" sheetId="75" r:id="rId49"/>
+    <sheet name="WellPressure" sheetId="118" r:id="rId50"/>
+    <sheet name="InitialPipelineCapacity" sheetId="66" r:id="rId51"/>
+    <sheet name="InitialPipelineDiameters" sheetId="119" r:id="rId52"/>
+    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId53"/>
+    <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId54"/>
+    <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId55"/>
+    <sheet name="ReuseMinimum" sheetId="126" r:id="rId56"/>
+    <sheet name="ReuseCapacity" sheetId="127" r:id="rId57"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId58"/>
+    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId59"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId60"/>
+    <sheet name="NodeCapacities" sheetId="107" r:id="rId61"/>
+    <sheet name="DisposalOperatingCapacity" sheetId="111" r:id="rId62"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId63"/>
+    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId64"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId65"/>
+    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId66"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId67"/>
+    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId68"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId69"/>
+    <sheet name="DisposalExpansionCost" sheetId="90" r:id="rId70"/>
+    <sheet name="DisposalCapacityIncrements" sheetId="79" r:id="rId71"/>
+    <sheet name="StorageExpansionCost" sheetId="91" r:id="rId72"/>
+    <sheet name="StorageCapacityIncrements" sheetId="81" r:id="rId73"/>
+    <sheet name="TreatmentExpansionCost" sheetId="92" r:id="rId74"/>
+    <sheet name="TreatmentCapacityIncrements" sheetId="87" r:id="rId75"/>
+    <sheet name="PipelineCapexDistanceBased" sheetId="89" r:id="rId76"/>
+    <sheet name="PipelineExpansionDistance" sheetId="103" r:id="rId77"/>
+    <sheet name="PipelineCapexCapacityBased" sheetId="101" r:id="rId78"/>
+    <sheet name="PipelineCapacityIncrements" sheetId="100" r:id="rId79"/>
+    <sheet name="PipelineDiameterValues" sheetId="93" r:id="rId80"/>
+    <sheet name="TreatmentEfficiency" sheetId="85" r:id="rId81"/>
+    <sheet name="RemovalEfficiency" sheetId="116" r:id="rId82"/>
+    <sheet name="DesalinationTechnologies" sheetId="112" r:id="rId83"/>
+    <sheet name="DesalinationSites" sheetId="114" r:id="rId84"/>
+    <sheet name="BeneficialReuseCredit" sheetId="128" r:id="rId85"/>
+    <sheet name="CompletionsPadOutsideSystem" sheetId="113" r:id="rId86"/>
+    <sheet name="Hydraulics" sheetId="95" r:id="rId87"/>
+    <sheet name="Economics" sheetId="99" r:id="rId88"/>
+    <sheet name="PadWaterQuality" sheetId="104" r:id="rId89"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="105" r:id="rId90"/>
+    <sheet name="PadStorageInitialWaterQuality" sheetId="106" r:id="rId91"/>
+    <sheet name="TreatmentExpansionLeadTime" sheetId="129" r:id="rId92"/>
+    <sheet name="DisposalExpansionLeadTime" sheetId="130" r:id="rId93"/>
+    <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId94"/>
+    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId95"/>
+    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId96"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId95"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="74" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="74">PipelineExpansionDistance!$O$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="76">PipelineExpansionDistance!$O$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -136,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3677" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3679" uniqueCount="311">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -1050,9 +1049,6 @@
     <t>Storage Sites to Beneficial Reuse Piping Arcs [-]</t>
   </si>
   <si>
-    <t>Storage Sites to Beneficial Reuse Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
-  </si>
-  <si>
     <t>Treatment to Storage Sites Trucking Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
   </si>
   <si>
@@ -1063,6 +1059,15 @@
   </si>
   <si>
     <t>pipeline_expansion_lead_time</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Beneficial Reuse Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Disposal Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Disposal Trucking Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
   </si>
 </sst>
 </file>
@@ -2074,271 +2079,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Overview"/>
-      <sheetName val="Schematic"/>
-      <sheetName val="Units"/>
-      <sheetName val="ProductionPads"/>
-      <sheetName val="ProductionTanks"/>
-      <sheetName val="CompletionsPads"/>
-      <sheetName val="SWDSites"/>
-      <sheetName val="FreshwaterSources"/>
-      <sheetName val="StorageSites"/>
-      <sheetName val="TreatmentSites"/>
-      <sheetName val="TreatmentTechnologies"/>
-      <sheetName val="ReuseOptions"/>
-      <sheetName val="NetworkNodes"/>
-      <sheetName val="PipelineDiameters"/>
-      <sheetName val="StorageCapacities"/>
-      <sheetName val="TreatmentCapacities"/>
-      <sheetName val="InjectionCapacities"/>
-      <sheetName val="PNA"/>
-      <sheetName val="CNA"/>
-      <sheetName val="CCA"/>
-      <sheetName val="NNA"/>
-      <sheetName val="NCA"/>
-      <sheetName val="NKA"/>
-      <sheetName val="NRA"/>
-      <sheetName val="NSA"/>
-      <sheetName val="SNA"/>
-      <sheetName val="FCA"/>
-      <sheetName val="RCA"/>
-      <sheetName val="RSA"/>
-      <sheetName val="SCA"/>
-      <sheetName val="RNA"/>
-      <sheetName val="PCT"/>
-      <sheetName val="FCT"/>
-      <sheetName val="PKT"/>
-      <sheetName val="CKT"/>
-      <sheetName val="CCT"/>
-      <sheetName val="CST"/>
-      <sheetName val="Elevation"/>
-      <sheetName val="CompletionsDemand"/>
-      <sheetName val="PadRates"/>
-      <sheetName val="FlowbackRates"/>
-      <sheetName val="WellPressure"/>
-      <sheetName val="InitialPipelineCapacity"/>
-      <sheetName val="InitialPipelineDiameters"/>
-      <sheetName val="InitialDisposalCapacity"/>
-      <sheetName val="InitialStorageCapacity"/>
-      <sheetName val="InitialTreatmentCapacity"/>
-      <sheetName val="FreshwaterSourcingAvailability"/>
-      <sheetName val="CompletionsPadStorage"/>
-      <sheetName val="PadOffloadingCapacity"/>
-      <sheetName val="NodeCapacities"/>
-      <sheetName val="DisposalOperatingCapacity"/>
-      <sheetName val="DisposalOperationalCost"/>
-      <sheetName val="TreatmentOperationalCost"/>
-      <sheetName val="ReuseOperationalCost"/>
-      <sheetName val="PipelineOperationalCost"/>
-      <sheetName val="FreshSourcingCost"/>
-      <sheetName val="TruckingHourlyCost"/>
-      <sheetName val="TruckingTime"/>
-      <sheetName val="DisposalExpansionCost"/>
-      <sheetName val="DisposalCapacityIncrements"/>
-      <sheetName val="StorageExpansionCost"/>
-      <sheetName val="StorageCapacityIncrements"/>
-      <sheetName val="TreatmentExpansionCost"/>
-      <sheetName val="TreatmentCapacityIncrements"/>
-      <sheetName val="PipelineCapexDistanceBased"/>
-      <sheetName val="PipelineExpansionDistance"/>
-      <sheetName val="PipelineCapexCapacityBased"/>
-      <sheetName val="PipelineCapacityIncrements"/>
-      <sheetName val="PipelineDiameterValues"/>
-      <sheetName val="TreatmentEfficiency"/>
-      <sheetName val="RemovalEfficiency"/>
-      <sheetName val="DesalinationTechnologies"/>
-      <sheetName val="DesalinationSites"/>
-      <sheetName val="CompletionsPadOutsideSystem"/>
-      <sheetName val="Hydraulics"/>
-      <sheetName val="Economics"/>
-      <sheetName val="PadWaterQuality"/>
-      <sheetName val="StorageInitialWaterQuality"/>
-      <sheetName val="PadStorageInitialWaterQuality"/>
-      <sheetName val="TreatmentExpansionLeadTime"/>
-      <sheetName val="DisposalExpansionLeadTime"/>
-      <sheetName val="StorageExpansionLeadTime"/>
-      <sheetName val="PipelineExpansionLeadTime_Dist"/>
-      <sheetName val="PipelineExpansionLeadTime_Capac"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>INDEX</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>VALUE</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>volume</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>bbl</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>distance</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>mile</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>diameter</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>inch</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>concentration</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>mg/liter</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>currency</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>USD</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>time</v>
-          </cell>
-          <cell r="B8" t="str">
-            <v>day</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>pressure</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>psi</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>elevation</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>foot</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>decision period</v>
-          </cell>
-          <cell r="B11" t="str">
-            <v>week</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-      <sheetData sheetId="74"/>
-      <sheetData sheetId="75"/>
-      <sheetData sheetId="76"/>
-      <sheetData sheetId="77"/>
-      <sheetData sheetId="78"/>
-      <sheetData sheetId="79"/>
-      <sheetData sheetId="80"/>
-      <sheetData sheetId="81"/>
-      <sheetData sheetId="82"/>
-      <sheetData sheetId="83"/>
-      <sheetData sheetId="84"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2641,7 +2381,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7574,14 +7314,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -7590,6 +7330,29 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D2FFAB-ECD3-4BD0-9D84-85E4DB7922BD}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6ED8ED-0A77-4974-A7C2-D2B875DA1401}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7768,7 +7531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F615298C-1D1C-4004-91BA-05C3C07D8B7C}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7899,7 +7662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8149,7 +7912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8238,85 +8001,6 @@
       <c r="D6" s="9">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37622F2B-1E4B-46C9-B210-3150CCBB5892}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="32"/>
-    </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="32"/>
-    </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8434,6 +8118,85 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37622F2B-1E4B-46C9-B210-3150CCBB5892}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="32"/>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A52059-0CB1-474F-ACFF-2997470BE1E9}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8477,7 +8240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7671FE8C-53C8-47E3-8F66-0CDFF992F8F0}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8496,7 +8259,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8529,8 +8292,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA0172C-9C06-4AFA-A735-EDA51E2D806D}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD3490E-F249-4CEC-A79A-88A8E596A07B}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -8552,22 +8338,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD3490E-F249-4CEC-A79A-88A8E596A07B}">
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D5E22A-C49D-4697-9262-298442E9AD18}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -8575,7 +8361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789E7D10-DA84-4E98-A491-162D17B0E3FF}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -9115,7 +8901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -9633,7 +9419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF4E1D-6CE0-4F02-8B9E-F2818C0A814C}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -13020,7 +12806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68666333-AE69-4574-92B2-6BE3A00DF612}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -13704,7 +13490,113 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FE18E-3C30-49FC-B6A0-0A6D3F02EBB0}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.28515625" style="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE870389-1558-469D-A4C0-FFF0CB6EF3E1}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -16993,7 +16885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE628BF-A05C-42C8-8EC7-63FF3B624ADC}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -19726,113 +19618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FE18E-3C30-49FC-B6A0-0A6D3F02EBB0}">
-  <dimension ref="A1:O15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="9.28515625" style="1"/>
-    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.28515625" style="1"/>
-    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AB3CAC-DE83-4E65-8BC7-386D18A19803}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -23979,7 +23765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24038,7 +23824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDF796A-A87C-4F37-A825-AF0AD18C802A}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24090,7 +23876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A13F53-E3AE-452E-A1A1-316A2C800322}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24150,7 +23936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71161610-124C-4EF0-9AD2-EA56457B2C52}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24174,7 +23960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93770ED0-6BFC-4696-92DB-4CEBACB9D35D}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24198,7 +23984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -25678,7 +25464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB793D-71C1-4CA2-A5D0-D94D2FB81D42}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -25739,116 +25525,6 @@
       <c r="B6" s="37">
         <v>800000</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
-  <sheetPr>
-    <tabColor rgb="FFD9C6FE"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Pad Offloading Capacity [bbl/week]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="35">
-        <v>210000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="35">
-        <v>210000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="35">
-        <v>210000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="37">
-        <v>210000</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D80780D-32E5-452A-A6C3-3B8E431097FA}">
-  <sheetPr>
-    <tabColor rgb="FFD9C6FE"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Node Capacity Capacity [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]", " (absence of node or empty cell signifies no max capacity)")</f>
-        <v>Table of Node Capacity Capacity [bbl/week] (absence of node or empty cell signifies no max capacity)</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25914,6 +25590,116 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
+  <sheetPr>
+    <tabColor rgb="FFD9C6FE"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Pad Offloading Capacity [bbl/week]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="35">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="35">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="35">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="37">
+        <v>210000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D80780D-32E5-452A-A6C3-3B8E431097FA}">
+  <sheetPr>
+    <tabColor rgb="FFD9C6FE"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Node Capacity Capacity [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]", " (absence of node or empty cell signifies no max capacity)")</f>
+        <v>Table of Node Capacity Capacity [bbl/week] (absence of node or empty cell signifies no max capacity)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F424B69F-B42E-4A8C-B24F-D4CE4D83DFA9}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -26595,7 +26381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -26655,7 +26441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7050C77-5C7B-4C97-8F2B-C60EA6AF1AED}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -26758,7 +26544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -26825,7 +26611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE24AD9-42B2-417F-BF2D-D0F067DA599C}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -26868,7 +26654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -26967,7 +26753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35585569-7889-4883-A327-3B12D4AB6358}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27218,7 +27004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27519,109 +27305,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E5CD4B-C8DB-4A49-956D-761D45563331}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$10, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),")]")</f>
-        <v>Table of Disposal Capacity Expansion Cost [USD/(bbl/week)]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="37">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982C988E-F277-4EB8-BD08-045871CAA4ED}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Disposal Capacity Expansion Increments [bbl/week]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="37">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -27675,6 +27358,109 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E5CD4B-C8DB-4A49-956D-761D45563331}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$10, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),")]")</f>
+        <v>Table of Disposal Capacity Expansion Cost [USD/(bbl/week)]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="37">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982C988E-F277-4EB8-BD08-045871CAA4ED}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Disposal Capacity Expansion Increments [bbl/week]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344AC655-401B-435E-9F3E-B4AFCEDA07DB}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27725,7 +27511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F26805-7F3D-4935-8D0C-80B2E9E9F409}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27768,7 +27554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D3944-A6F1-468B-A756-A99C077811C6}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27867,7 +27653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6DB070-53D7-4763-B1D6-04233A007F0E}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27928,7 +27714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C902C13-E391-4A34-8851-63FF84EE5034}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27971,7 +27757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBA4E88-E142-4CAA-9941-4EFBE822A9B8}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -35087,7 +34873,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB463F82-A1C0-450F-A6BA-E327D67D2CCA}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -35144,7 +34930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DDE49D4-5953-41A3-9445-43C5CEE52016}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -35180,153 +34966,6 @@
       <c r="B3" s="37">
         <v>0</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451B8273-C388-463D-8494-0D66D9ED9BA0}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Diameters [",VLOOKUP("diameter", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Pipeline Diameters [inch]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="37">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45C9D-7A15-425D-8487-B88B27280274}">
-  <sheetPr>
-    <tabColor rgb="FFAFF3DE"/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>280</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="80" t="s">
-        <v>277</v>
-      </c>
-      <c r="C3" s="32">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="80" t="s">
-        <v>277</v>
-      </c>
-      <c r="C4" s="32">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="80" t="s">
-        <v>278</v>
-      </c>
-      <c r="C5" s="32">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="81" t="s">
-        <v>278</v>
-      </c>
-      <c r="C6" s="33">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35414,6 +35053,153 @@
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451B8273-C388-463D-8494-0D66D9ED9BA0}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pipeline Diameters [",VLOOKUP("diameter", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Pipeline Diameters [inch]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45C9D-7A15-425D-8487-B88B27280274}">
+  <sheetPr>
+    <tabColor rgb="FFAFF3DE"/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="79" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" s="32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="80" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" s="32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="81" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A32EEB0-CDB8-48FA-AC3A-32F164C0112D}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35508,7 +35294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CCDB1D-7C9B-45C0-BC80-50ECEB2FE439}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35556,7 +35342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805001D5-70DF-464C-8122-7D31EBC77774}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35620,7 +35406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C085ECA6-7B3E-4F26-A39A-70D9F45A71B6}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35644,7 +35430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D5E840-A652-4014-8BA7-131503FECE29}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35708,7 +35494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97A568C-E2FB-4ADF-84D0-ABF3E0446F9A}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35756,7 +35542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB07E06-ED03-4572-9B3E-05DAA3F2CF42}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35804,7 +35590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23C97C0-70AD-4A71-BE9C-0931EDC97CA5}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -36049,149 +35835,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485401B3-8B00-41A4-BDC3-322B62874F13}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [",VLOOKUP("concentration", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Initial Water Quality at Storage [mg/liter]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="48">
-        <v>150000</v>
-      </c>
-      <c r="C3" s="48">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="B4" s="50">
-        <v>150000</v>
-      </c>
-      <c r="C4" s="50">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C5F8D1-3580-447F-A30D-0D2BFC2160E3}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Completions Pad Storage [",VLOOKUP("concentration", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Initial Water Quality at Completions Pad Storage [mg/liter]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="49">
-        <v>150000</v>
-      </c>
-      <c r="C3" s="49">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="49">
-        <v>150000</v>
-      </c>
-      <c r="C4" s="49">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="49">
-        <v>150000</v>
-      </c>
-      <c r="C5" s="49">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="50">
-        <v>150000</v>
-      </c>
-      <c r="C6" s="50">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -36242,6 +35885,149 @@
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485401B3-8B00-41A4-BDC3-322B62874F13}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [",VLOOKUP("concentration", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Initial Water Quality at Storage [mg/liter]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="48">
+        <v>150000</v>
+      </c>
+      <c r="C3" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" s="50">
+        <v>150000</v>
+      </c>
+      <c r="C4" s="50">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C5F8D1-3580-447F-A30D-0D2BFC2160E3}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Completions Pad Storage [",VLOOKUP("concentration", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Initial Water Quality at Completions Pad Storage [mg/liter]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="49">
+        <v>150000</v>
+      </c>
+      <c r="C3" s="49">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="49">
+        <v>150000</v>
+      </c>
+      <c r="C4" s="49">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="49">
+        <v>150000</v>
+      </c>
+      <c r="C5" s="49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="50">
+        <v>150000</v>
+      </c>
+      <c r="C6" s="50">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DB2954-C948-47D3-8551-66A5E543A667}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -36249,14 +36035,14 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Treatment Expansion Lead Time [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s]")</f>
+        <f>_xlfn.CONCAT( "Table of Treatment Expansion Lead Time [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
         <v>Table of Treatment Expansion Lead Time [weeks]</v>
       </c>
       <c r="B1" s="1"/>
@@ -36282,7 +36068,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DCF108-65D2-4920-AF63-41DE3C60BC9F}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -36290,14 +36076,14 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Disposal Expansion Lead Time [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s]")</f>
+        <f>_xlfn.CONCAT( "Table of Disposal Expansion Lead Time [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
         <v>Table of Disposal Expansion Lead Time [weeks]</v>
       </c>
       <c r="B1" s="1"/>
@@ -36308,7 +36094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E838BDDE-4D1E-4BCC-805C-186192CF51E1}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -36316,15 +36102,15 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s]")</f>
-        <v>Table of Pipeline Expansion Lead Time - Distance Based [weeks]</v>
+        <f>_xlfn.CONCAT( "Table of Storage Expansion Lead Time [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
+        <v>Table of Storage Expansion Lead Time [weeks]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -36334,7 +36120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E009F48F-F710-4F4F-876A-C3ABC3B5BD14}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -36342,7 +36128,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36352,7 +36138,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s/",VLOOKUP("distance", [1]Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s/",VLOOKUP("distance", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Pipeline Expansion Lead Time - Distance Based [weeks/mile]</v>
       </c>
     </row>
@@ -36366,7 +36152,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B3" s="42">
         <v>0</v>
@@ -36377,23 +36163,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431BFE9B-561C-4E4E-9282-73406F634D63}">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s]")</f>
-        <v>Table of Pipeline Expansion Lead Time - Distance Based [weeks]</v>
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Capacity Based [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
+        <v>Table of Pipeline Expansion Lead Time - Capacity Based [weeks]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>

</xml_diff>

<commit_message>
Support RKA and RKT arcs and beneficial reuse processing cost in strategic model (#276)
* Support RKA and RKT arcs in strategic model

* Implement beneficial reuse processing cost

* Fix tests
</commit_message>
<xml_diff>
--- a/pareto/tests/strategic_small_case_study_load_removaleff.xlsx
+++ b/pareto/tests/strategic_small_case_study_load_removaleff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089CE096-EC15-48B1-B6C8-83BE79DDD390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24072696-4473-4D60-B5E6-9C502F048AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="88" activeTab="93" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -47,73 +47,73 @@
     <sheet name="SCA" sheetId="97" r:id="rId32"/>
     <sheet name="RNA" sheetId="62" r:id="rId33"/>
     <sheet name="ROA" sheetId="122" r:id="rId34"/>
-    <sheet name="PCT" sheetId="42" r:id="rId35"/>
-    <sheet name="FCT" sheetId="70" r:id="rId36"/>
-    <sheet name="PKT" sheetId="43" r:id="rId37"/>
-    <sheet name="CKT" sheetId="44" r:id="rId38"/>
-    <sheet name="CCT" sheetId="74" r:id="rId39"/>
-    <sheet name="CST" sheetId="64" r:id="rId40"/>
-    <sheet name="RST" sheetId="123" r:id="rId41"/>
-    <sheet name="ROT" sheetId="124" r:id="rId42"/>
-    <sheet name="SOT" sheetId="125" r:id="rId43"/>
-    <sheet name="Elevation" sheetId="117" r:id="rId44"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId45"/>
-    <sheet name="PadRates" sheetId="65" r:id="rId46"/>
-    <sheet name="FlowbackRates" sheetId="75" r:id="rId47"/>
-    <sheet name="WellPressure" sheetId="118" r:id="rId48"/>
-    <sheet name="InitialPipelineCapacity" sheetId="66" r:id="rId49"/>
-    <sheet name="InitialPipelineDiameters" sheetId="119" r:id="rId50"/>
-    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId51"/>
-    <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId52"/>
-    <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId53"/>
-    <sheet name="ReuseMinimum" sheetId="126" r:id="rId54"/>
-    <sheet name="ReuseCapacity" sheetId="127" r:id="rId55"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId56"/>
-    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId57"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId58"/>
-    <sheet name="NodeCapacities" sheetId="107" r:id="rId59"/>
-    <sheet name="DisposalOperatingCapacity" sheetId="111" r:id="rId60"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId61"/>
-    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId62"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId63"/>
-    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId64"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId65"/>
-    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId66"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId67"/>
-    <sheet name="DisposalExpansionCost" sheetId="90" r:id="rId68"/>
-    <sheet name="DisposalCapacityIncrements" sheetId="79" r:id="rId69"/>
-    <sheet name="StorageExpansionCost" sheetId="91" r:id="rId70"/>
-    <sheet name="StorageCapacityIncrements" sheetId="81" r:id="rId71"/>
-    <sheet name="TreatmentExpansionCost" sheetId="92" r:id="rId72"/>
-    <sheet name="TreatmentCapacityIncrements" sheetId="87" r:id="rId73"/>
-    <sheet name="PipelineCapexDistanceBased" sheetId="89" r:id="rId74"/>
-    <sheet name="PipelineExpansionDistance" sheetId="103" r:id="rId75"/>
-    <sheet name="PipelineCapexCapacityBased" sheetId="101" r:id="rId76"/>
-    <sheet name="PipelineCapacityIncrements" sheetId="100" r:id="rId77"/>
-    <sheet name="PipelineDiameterValues" sheetId="93" r:id="rId78"/>
-    <sheet name="TreatmentEfficiency" sheetId="85" r:id="rId79"/>
-    <sheet name="RemovalEfficiency" sheetId="116" r:id="rId80"/>
-    <sheet name="DesalinationTechnologies" sheetId="112" r:id="rId81"/>
-    <sheet name="DesalinationSites" sheetId="114" r:id="rId82"/>
-    <sheet name="BeneficialReuseCredit" sheetId="128" r:id="rId83"/>
-    <sheet name="CompletionsPadOutsideSystem" sheetId="113" r:id="rId84"/>
-    <sheet name="Hydraulics" sheetId="95" r:id="rId85"/>
-    <sheet name="Economics" sheetId="99" r:id="rId86"/>
-    <sheet name="PadWaterQuality" sheetId="104" r:id="rId87"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="105" r:id="rId88"/>
-    <sheet name="PadStorageInitialWaterQuality" sheetId="106" r:id="rId89"/>
-    <sheet name="TreatmentExpansionLeadTime" sheetId="129" r:id="rId90"/>
-    <sheet name="DisposalExpansionLeadTime" sheetId="130" r:id="rId91"/>
-    <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId92"/>
-    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId93"/>
-    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId94"/>
+    <sheet name="RKA" sheetId="134" r:id="rId35"/>
+    <sheet name="PCT" sheetId="42" r:id="rId36"/>
+    <sheet name="FCT" sheetId="70" r:id="rId37"/>
+    <sheet name="PKT" sheetId="43" r:id="rId38"/>
+    <sheet name="CKT" sheetId="44" r:id="rId39"/>
+    <sheet name="CCT" sheetId="74" r:id="rId40"/>
+    <sheet name="CST" sheetId="64" r:id="rId41"/>
+    <sheet name="RST" sheetId="123" r:id="rId42"/>
+    <sheet name="ROT" sheetId="124" r:id="rId43"/>
+    <sheet name="SOT" sheetId="125" r:id="rId44"/>
+    <sheet name="RKT" sheetId="135" r:id="rId45"/>
+    <sheet name="Elevation" sheetId="117" r:id="rId46"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId47"/>
+    <sheet name="PadRates" sheetId="65" r:id="rId48"/>
+    <sheet name="FlowbackRates" sheetId="75" r:id="rId49"/>
+    <sheet name="WellPressure" sheetId="118" r:id="rId50"/>
+    <sheet name="InitialPipelineCapacity" sheetId="66" r:id="rId51"/>
+    <sheet name="InitialPipelineDiameters" sheetId="119" r:id="rId52"/>
+    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId53"/>
+    <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId54"/>
+    <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId55"/>
+    <sheet name="ReuseMinimum" sheetId="126" r:id="rId56"/>
+    <sheet name="ReuseCapacity" sheetId="127" r:id="rId57"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId58"/>
+    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId59"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId60"/>
+    <sheet name="NodeCapacities" sheetId="107" r:id="rId61"/>
+    <sheet name="DisposalOperatingCapacity" sheetId="111" r:id="rId62"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId63"/>
+    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId64"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId65"/>
+    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId66"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId67"/>
+    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId68"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId69"/>
+    <sheet name="DisposalExpansionCost" sheetId="90" r:id="rId70"/>
+    <sheet name="DisposalCapacityIncrements" sheetId="79" r:id="rId71"/>
+    <sheet name="StorageExpansionCost" sheetId="91" r:id="rId72"/>
+    <sheet name="StorageCapacityIncrements" sheetId="81" r:id="rId73"/>
+    <sheet name="TreatmentExpansionCost" sheetId="92" r:id="rId74"/>
+    <sheet name="TreatmentCapacityIncrements" sheetId="87" r:id="rId75"/>
+    <sheet name="PipelineCapexDistanceBased" sheetId="89" r:id="rId76"/>
+    <sheet name="PipelineExpansionDistance" sheetId="103" r:id="rId77"/>
+    <sheet name="PipelineCapexCapacityBased" sheetId="101" r:id="rId78"/>
+    <sheet name="PipelineCapacityIncrements" sheetId="100" r:id="rId79"/>
+    <sheet name="PipelineDiameterValues" sheetId="93" r:id="rId80"/>
+    <sheet name="TreatmentEfficiency" sheetId="85" r:id="rId81"/>
+    <sheet name="RemovalEfficiency" sheetId="116" r:id="rId82"/>
+    <sheet name="DesalinationTechnologies" sheetId="112" r:id="rId83"/>
+    <sheet name="DesalinationSites" sheetId="114" r:id="rId84"/>
+    <sheet name="BeneficialReuseCost" sheetId="136" r:id="rId85"/>
+    <sheet name="BeneficialReuseCredit" sheetId="128" r:id="rId86"/>
+    <sheet name="CompletionsPadOutsideSystem" sheetId="113" r:id="rId87"/>
+    <sheet name="Hydraulics" sheetId="95" r:id="rId88"/>
+    <sheet name="Economics" sheetId="99" r:id="rId89"/>
+    <sheet name="PadWaterQuality" sheetId="104" r:id="rId90"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="105" r:id="rId91"/>
+    <sheet name="PadStorageInitialWaterQuality" sheetId="106" r:id="rId92"/>
+    <sheet name="TreatmentExpansionLeadTime" sheetId="129" r:id="rId93"/>
+    <sheet name="DisposalExpansionLeadTime" sheetId="130" r:id="rId94"/>
+    <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId95"/>
+    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId96"/>
+    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId97"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId95"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="74" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="74">PipelineExpansionDistance!$O$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="76">PipelineExpansionDistance!$O$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3677" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3679" uniqueCount="311">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -1050,9 +1050,6 @@
     <t>Storage Sites to Beneficial Reuse Piping Arcs [-]</t>
   </si>
   <si>
-    <t>Storage Sites to Beneficial Reuse Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
-  </si>
-  <si>
     <t>Treatment to Storage Sites Trucking Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
   </si>
   <si>
@@ -1063,6 +1060,15 @@
   </si>
   <si>
     <t>pipeline_expansion_lead_time</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Beneficial Reuse Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Disposal Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Disposal Trucking Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
   </si>
 </sst>
 </file>
@@ -2074,271 +2080,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Overview"/>
-      <sheetName val="Schematic"/>
-      <sheetName val="Units"/>
-      <sheetName val="ProductionPads"/>
-      <sheetName val="ProductionTanks"/>
-      <sheetName val="CompletionsPads"/>
-      <sheetName val="SWDSites"/>
-      <sheetName val="FreshwaterSources"/>
-      <sheetName val="StorageSites"/>
-      <sheetName val="TreatmentSites"/>
-      <sheetName val="TreatmentTechnologies"/>
-      <sheetName val="ReuseOptions"/>
-      <sheetName val="NetworkNodes"/>
-      <sheetName val="PipelineDiameters"/>
-      <sheetName val="StorageCapacities"/>
-      <sheetName val="TreatmentCapacities"/>
-      <sheetName val="InjectionCapacities"/>
-      <sheetName val="PNA"/>
-      <sheetName val="CNA"/>
-      <sheetName val="CCA"/>
-      <sheetName val="NNA"/>
-      <sheetName val="NCA"/>
-      <sheetName val="NKA"/>
-      <sheetName val="NRA"/>
-      <sheetName val="NSA"/>
-      <sheetName val="SNA"/>
-      <sheetName val="FCA"/>
-      <sheetName val="RCA"/>
-      <sheetName val="RSA"/>
-      <sheetName val="SCA"/>
-      <sheetName val="RNA"/>
-      <sheetName val="PCT"/>
-      <sheetName val="FCT"/>
-      <sheetName val="PKT"/>
-      <sheetName val="CKT"/>
-      <sheetName val="CCT"/>
-      <sheetName val="CST"/>
-      <sheetName val="Elevation"/>
-      <sheetName val="CompletionsDemand"/>
-      <sheetName val="PadRates"/>
-      <sheetName val="FlowbackRates"/>
-      <sheetName val="WellPressure"/>
-      <sheetName val="InitialPipelineCapacity"/>
-      <sheetName val="InitialPipelineDiameters"/>
-      <sheetName val="InitialDisposalCapacity"/>
-      <sheetName val="InitialStorageCapacity"/>
-      <sheetName val="InitialTreatmentCapacity"/>
-      <sheetName val="FreshwaterSourcingAvailability"/>
-      <sheetName val="CompletionsPadStorage"/>
-      <sheetName val="PadOffloadingCapacity"/>
-      <sheetName val="NodeCapacities"/>
-      <sheetName val="DisposalOperatingCapacity"/>
-      <sheetName val="DisposalOperationalCost"/>
-      <sheetName val="TreatmentOperationalCost"/>
-      <sheetName val="ReuseOperationalCost"/>
-      <sheetName val="PipelineOperationalCost"/>
-      <sheetName val="FreshSourcingCost"/>
-      <sheetName val="TruckingHourlyCost"/>
-      <sheetName val="TruckingTime"/>
-      <sheetName val="DisposalExpansionCost"/>
-      <sheetName val="DisposalCapacityIncrements"/>
-      <sheetName val="StorageExpansionCost"/>
-      <sheetName val="StorageCapacityIncrements"/>
-      <sheetName val="TreatmentExpansionCost"/>
-      <sheetName val="TreatmentCapacityIncrements"/>
-      <sheetName val="PipelineCapexDistanceBased"/>
-      <sheetName val="PipelineExpansionDistance"/>
-      <sheetName val="PipelineCapexCapacityBased"/>
-      <sheetName val="PipelineCapacityIncrements"/>
-      <sheetName val="PipelineDiameterValues"/>
-      <sheetName val="TreatmentEfficiency"/>
-      <sheetName val="RemovalEfficiency"/>
-      <sheetName val="DesalinationTechnologies"/>
-      <sheetName val="DesalinationSites"/>
-      <sheetName val="CompletionsPadOutsideSystem"/>
-      <sheetName val="Hydraulics"/>
-      <sheetName val="Economics"/>
-      <sheetName val="PadWaterQuality"/>
-      <sheetName val="StorageInitialWaterQuality"/>
-      <sheetName val="PadStorageInitialWaterQuality"/>
-      <sheetName val="TreatmentExpansionLeadTime"/>
-      <sheetName val="DisposalExpansionLeadTime"/>
-      <sheetName val="StorageExpansionLeadTime"/>
-      <sheetName val="PipelineExpansionLeadTime_Dist"/>
-      <sheetName val="PipelineExpansionLeadTime_Capac"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>INDEX</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>VALUE</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>volume</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>bbl</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>distance</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>mile</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>diameter</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>inch</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>concentration</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>mg/liter</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>currency</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>USD</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>time</v>
-          </cell>
-          <cell r="B8" t="str">
-            <v>day</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>pressure</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>psi</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>elevation</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>foot</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>decision period</v>
-          </cell>
-          <cell r="B11" t="str">
-            <v>week</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-      <sheetData sheetId="74"/>
-      <sheetData sheetId="75"/>
-      <sheetData sheetId="76"/>
-      <sheetData sheetId="77"/>
-      <sheetData sheetId="78"/>
-      <sheetData sheetId="79"/>
-      <sheetData sheetId="80"/>
-      <sheetData sheetId="81"/>
-      <sheetData sheetId="82"/>
-      <sheetData sheetId="83"/>
-      <sheetData sheetId="84"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2641,7 +2382,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7574,14 +7315,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -7590,6 +7331,29 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D2FFAB-ECD3-4BD0-9D84-85E4DB7922BD}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6ED8ED-0A77-4974-A7C2-D2B875DA1401}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7768,7 +7532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F615298C-1D1C-4004-91BA-05C3C07D8B7C}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7899,7 +7663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8149,7 +7913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8238,85 +8002,6 @@
       <c r="D6" s="9">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37622F2B-1E4B-46C9-B210-3150CCBB5892}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="32"/>
-    </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="32"/>
-    </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8434,6 +8119,85 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37622F2B-1E4B-46C9-B210-3150CCBB5892}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="32"/>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A52059-0CB1-474F-ACFF-2997470BE1E9}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8477,7 +8241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7671FE8C-53C8-47E3-8F66-0CDFF992F8F0}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8496,7 +8260,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8529,8 +8293,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA0172C-9C06-4AFA-A735-EDA51E2D806D}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD3490E-F249-4CEC-A79A-88A8E596A07B}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -8552,22 +8339,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD3490E-F249-4CEC-A79A-88A8E596A07B}">
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D5E22A-C49D-4697-9262-298442E9AD18}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -8575,7 +8362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789E7D10-DA84-4E98-A491-162D17B0E3FF}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -9115,7 +8902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -9633,7 +9420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF4E1D-6CE0-4F02-8B9E-F2818C0A814C}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -13020,7 +12807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68666333-AE69-4574-92B2-6BE3A00DF612}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -13704,7 +13491,113 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FE18E-3C30-49FC-B6A0-0A6D3F02EBB0}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.28515625" style="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE870389-1558-469D-A4C0-FFF0CB6EF3E1}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -16993,7 +16886,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE628BF-A05C-42C8-8EC7-63FF3B624ADC}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -19726,113 +19619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FE18E-3C30-49FC-B6A0-0A6D3F02EBB0}">
-  <dimension ref="A1:O15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="9.28515625" style="1"/>
-    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.28515625" style="1"/>
-    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AB3CAC-DE83-4E65-8BC7-386D18A19803}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -23979,7 +23766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24038,7 +23825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDF796A-A87C-4F37-A825-AF0AD18C802A}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24090,7 +23877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A13F53-E3AE-452E-A1A1-316A2C800322}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24150,7 +23937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71161610-124C-4EF0-9AD2-EA56457B2C52}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24174,7 +23961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93770ED0-6BFC-4696-92DB-4CEBACB9D35D}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24198,7 +23985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -25678,7 +25465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB793D-71C1-4CA2-A5D0-D94D2FB81D42}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -25739,116 +25526,6 @@
       <c r="B6" s="37">
         <v>800000</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
-  <sheetPr>
-    <tabColor rgb="FFD9C6FE"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Pad Offloading Capacity [bbl/week]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="35">
-        <v>210000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="35">
-        <v>210000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="35">
-        <v>210000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="37">
-        <v>210000</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D80780D-32E5-452A-A6C3-3B8E431097FA}">
-  <sheetPr>
-    <tabColor rgb="FFD9C6FE"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Node Capacity Capacity [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]", " (absence of node or empty cell signifies no max capacity)")</f>
-        <v>Table of Node Capacity Capacity [bbl/week] (absence of node or empty cell signifies no max capacity)</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25914,6 +25591,116 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
+  <sheetPr>
+    <tabColor rgb="FFD9C6FE"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Pad Offloading Capacity [bbl/week]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="35">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="35">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="35">
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="37">
+        <v>210000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D80780D-32E5-452A-A6C3-3B8E431097FA}">
+  <sheetPr>
+    <tabColor rgb="FFD9C6FE"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Node Capacity Capacity [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]", " (absence of node or empty cell signifies no max capacity)")</f>
+        <v>Table of Node Capacity Capacity [bbl/week] (absence of node or empty cell signifies no max capacity)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F424B69F-B42E-4A8C-B24F-D4CE4D83DFA9}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -26595,7 +26382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -26655,7 +26442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7050C77-5C7B-4C97-8F2B-C60EA6AF1AED}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -26758,7 +26545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -26825,7 +26612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE24AD9-42B2-417F-BF2D-D0F067DA599C}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -26868,7 +26655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -26967,7 +26754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35585569-7889-4883-A327-3B12D4AB6358}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27218,7 +27005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27519,109 +27306,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E5CD4B-C8DB-4A49-956D-761D45563331}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$10, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),")]")</f>
-        <v>Table of Disposal Capacity Expansion Cost [USD/(bbl/week)]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="37">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982C988E-F277-4EB8-BD08-045871CAA4ED}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Disposal Capacity Expansion Increments [bbl/week]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="37">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -27675,6 +27359,109 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E5CD4B-C8DB-4A49-956D-761D45563331}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$10, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),")]")</f>
+        <v>Table of Disposal Capacity Expansion Cost [USD/(bbl/week)]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="37">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982C988E-F277-4EB8-BD08-045871CAA4ED}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$10, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Disposal Capacity Expansion Increments [bbl/week]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344AC655-401B-435E-9F3E-B4AFCEDA07DB}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27725,7 +27512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F26805-7F3D-4935-8D0C-80B2E9E9F409}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27768,7 +27555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D3944-A6F1-468B-A756-A99C077811C6}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27867,7 +27654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6DB070-53D7-4763-B1D6-04233A007F0E}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27928,7 +27715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C902C13-E391-4A34-8851-63FF84EE5034}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -27971,7 +27758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBA4E88-E142-4CAA-9941-4EFBE822A9B8}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -35087,7 +34874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB463F82-A1C0-450F-A6BA-E327D67D2CCA}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -35144,7 +34931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DDE49D4-5953-41A3-9445-43C5CEE52016}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -35180,153 +34967,6 @@
       <c r="B3" s="37">
         <v>0</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451B8273-C388-463D-8494-0D66D9ED9BA0}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Diameters [",VLOOKUP("diameter", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Pipeline Diameters [inch]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="37">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45C9D-7A15-425D-8487-B88B27280274}">
-  <sheetPr>
-    <tabColor rgb="FFAFF3DE"/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>280</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="80" t="s">
-        <v>277</v>
-      </c>
-      <c r="C3" s="32">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="80" t="s">
-        <v>277</v>
-      </c>
-      <c r="C4" s="32">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="80" t="s">
-        <v>278</v>
-      </c>
-      <c r="C5" s="32">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="81" t="s">
-        <v>278</v>
-      </c>
-      <c r="C6" s="33">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35414,6 +35054,153 @@
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451B8273-C388-463D-8494-0D66D9ED9BA0}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pipeline Diameters [",VLOOKUP("diameter", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Pipeline Diameters [inch]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45C9D-7A15-425D-8487-B88B27280274}">
+  <sheetPr>
+    <tabColor rgb="FFAFF3DE"/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="79" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" s="32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" s="32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="80" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" s="32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="81" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A32EEB0-CDB8-48FA-AC3A-32F164C0112D}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35508,7 +35295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CCDB1D-7C9B-45C0-BC80-50ECEB2FE439}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35556,7 +35343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805001D5-70DF-464C-8122-7D31EBC77774}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35620,7 +35407,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93D2995-5E8F-4CB1-BE39-9D6C29509556}">
+  <sheetPr>
+    <tabColor rgb="FFAFF3DE"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>CONCATENATE( "Table with processing cost for sending water to beneficial reuse [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table with processing cost for sending water to beneficial reuse [USD/bbl]</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C085ECA6-7B3E-4F26-A39A-70D9F45A71B6}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35628,13 +35442,16 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
+      <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table with credit received for sending water to beneficial reuse [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table with credit received for sending water to beneficial reuse [USD/bbl]</v>
       </c>
@@ -35644,7 +35461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D5E840-A652-4014-8BA7-131503FECE29}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35708,7 +35525,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97A568C-E2FB-4ADF-84D0-ABF3E0446F9A}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35756,7 +35573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB07E06-ED03-4572-9B3E-05DAA3F2CF42}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -35796,397 +35613,6 @@
         <v>231</v>
       </c>
       <c r="B4" s="37">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23C97C0-70AD-4A71-BE9C-0931EDC97CA5}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="48">
-        <v>142277</v>
-      </c>
-      <c r="C3" s="48">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="49">
-        <v>140998</v>
-      </c>
-      <c r="C4" s="49">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="49">
-        <v>172490.2</v>
-      </c>
-      <c r="C5" s="49">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="49">
-        <v>257547</v>
-      </c>
-      <c r="C6" s="49">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="49">
-        <v>241833.8</v>
-      </c>
-      <c r="C7" s="48">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="49">
-        <v>188503.7</v>
-      </c>
-      <c r="C8" s="49">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="49">
-        <v>146716</v>
-      </c>
-      <c r="C9" s="49">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="49">
-        <v>216563</v>
-      </c>
-      <c r="C10" s="49">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="49">
-        <v>150626</v>
-      </c>
-      <c r="C11" s="48">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12" s="49">
-        <v>247061</v>
-      </c>
-      <c r="C12" s="49">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="49">
-        <v>180968</v>
-      </c>
-      <c r="C13" s="49">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="49">
-        <v>195584</v>
-      </c>
-      <c r="C14" s="49">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="49">
-        <v>148655</v>
-      </c>
-      <c r="C15" s="49">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="B16" s="49">
-        <v>185369</v>
-      </c>
-      <c r="C16" s="49">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" s="108">
-        <v>222724</v>
-      </c>
-      <c r="C17" s="49">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="49">
-        <v>165376</v>
-      </c>
-      <c r="C18" s="48">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" s="49">
-        <v>240977</v>
-      </c>
-      <c r="C19" s="49">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B20" s="49">
-        <v>192794</v>
-      </c>
-      <c r="C20" s="49">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="50">
-        <v>216769</v>
-      </c>
-      <c r="C21" s="49">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485401B3-8B00-41A4-BDC3-322B62874F13}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [",VLOOKUP("concentration", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Initial Water Quality at Storage [mg/liter]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="48">
-        <v>150000</v>
-      </c>
-      <c r="C3" s="48">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="B4" s="50">
-        <v>150000</v>
-      </c>
-      <c r="C4" s="50">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C5F8D1-3580-447F-A30D-0D2BFC2160E3}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Completions Pad Storage [",VLOOKUP("concentration", Units!$A$2:$B$10, 2, FALSE),"]")</f>
-        <v>Table of Initial Water Quality at Completions Pad Storage [mg/liter]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="49">
-        <v>150000</v>
-      </c>
-      <c r="C3" s="49">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="49">
-        <v>150000</v>
-      </c>
-      <c r="C4" s="49">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="49">
-        <v>150000</v>
-      </c>
-      <c r="C5" s="49">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="50">
-        <v>150000</v>
-      </c>
-      <c r="C6" s="50">
         <v>20</v>
       </c>
     </row>
@@ -36242,6 +35668,397 @@
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23C97C0-70AD-4A71-BE9C-0931EDC97CA5}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="48">
+        <v>142277</v>
+      </c>
+      <c r="C3" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="49">
+        <v>140998</v>
+      </c>
+      <c r="C4" s="49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="49">
+        <v>172490.2</v>
+      </c>
+      <c r="C5" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="49">
+        <v>257547</v>
+      </c>
+      <c r="C6" s="49">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="49">
+        <v>241833.8</v>
+      </c>
+      <c r="C7" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="49">
+        <v>188503.7</v>
+      </c>
+      <c r="C8" s="49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="49">
+        <v>146716</v>
+      </c>
+      <c r="C9" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="49">
+        <v>216563</v>
+      </c>
+      <c r="C10" s="49">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="49">
+        <v>150626</v>
+      </c>
+      <c r="C11" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="49">
+        <v>247061</v>
+      </c>
+      <c r="C12" s="49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="49">
+        <v>180968</v>
+      </c>
+      <c r="C13" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="49">
+        <v>195584</v>
+      </c>
+      <c r="C14" s="49">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="49">
+        <v>148655</v>
+      </c>
+      <c r="C15" s="49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="49">
+        <v>185369</v>
+      </c>
+      <c r="C16" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="108">
+        <v>222724</v>
+      </c>
+      <c r="C17" s="49">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="49">
+        <v>165376</v>
+      </c>
+      <c r="C18" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="49">
+        <v>240977</v>
+      </c>
+      <c r="C19" s="49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="49">
+        <v>192794</v>
+      </c>
+      <c r="C20" s="49">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="50">
+        <v>216769</v>
+      </c>
+      <c r="C21" s="49">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485401B3-8B00-41A4-BDC3-322B62874F13}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [",VLOOKUP("concentration", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Initial Water Quality at Storage [mg/liter]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="48">
+        <v>150000</v>
+      </c>
+      <c r="C3" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" s="50">
+        <v>150000</v>
+      </c>
+      <c r="C4" s="50">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C5F8D1-3580-447F-A30D-0D2BFC2160E3}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Completions Pad Storage [",VLOOKUP("concentration", Units!$A$2:$B$10, 2, FALSE),"]")</f>
+        <v>Table of Initial Water Quality at Completions Pad Storage [mg/liter]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="49">
+        <v>150000</v>
+      </c>
+      <c r="C3" s="49">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="49">
+        <v>150000</v>
+      </c>
+      <c r="C4" s="49">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="49">
+        <v>150000</v>
+      </c>
+      <c r="C5" s="49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="50">
+        <v>150000</v>
+      </c>
+      <c r="C6" s="50">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DB2954-C948-47D3-8551-66A5E543A667}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -36249,14 +36066,14 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Treatment Expansion Lead Time [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s]")</f>
+        <f>_xlfn.CONCAT( "Table of Treatment Expansion Lead Time [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
         <v>Table of Treatment Expansion Lead Time [weeks]</v>
       </c>
       <c r="B1" s="1"/>
@@ -36282,7 +36099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DCF108-65D2-4920-AF63-41DE3C60BC9F}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -36290,14 +36107,14 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Disposal Expansion Lead Time [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s]")</f>
+        <f>_xlfn.CONCAT( "Table of Disposal Expansion Lead Time [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
         <v>Table of Disposal Expansion Lead Time [weeks]</v>
       </c>
       <c r="B1" s="1"/>
@@ -36308,7 +36125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E838BDDE-4D1E-4BCC-805C-186192CF51E1}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -36316,15 +36133,15 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s]")</f>
-        <v>Table of Pipeline Expansion Lead Time - Distance Based [weeks]</v>
+        <f>_xlfn.CONCAT( "Table of Storage Expansion Lead Time [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
+        <v>Table of Storage Expansion Lead Time [weeks]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -36334,7 +36151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E009F48F-F710-4F4F-876A-C3ABC3B5BD14}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -36342,7 +36159,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36352,7 +36169,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s/",VLOOKUP("distance", [1]Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s/",VLOOKUP("distance", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Pipeline Expansion Lead Time - Distance Based [weeks/mile]</v>
       </c>
     </row>
@@ -36366,7 +36183,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B3" s="42">
         <v>0</v>
@@ -36377,23 +36194,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431BFE9B-561C-4E4E-9282-73406F634D63}">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s]")</f>
-        <v>Table of Pipeline Expansion Lead Time - Distance Based [weeks]</v>
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Capacity Based [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
+        <v>Table of Pipeline Expansion Lead Time - Capacity Based [weeks]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>

</xml_diff>